<commit_message>
android app folder with config file
</commit_message>
<xml_diff>
--- a/Summary_2022-08-28.xlsx
+++ b/Summary_2022-08-28.xlsx
@@ -441,19 +441,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.0241</v>
+        <v>-0.007900000000000001</v>
       </c>
       <c r="C2">
-        <v>0.0241</v>
+        <v>-0.007900000000000001</v>
       </c>
       <c r="D2">
-        <v>0.0328</v>
+        <v>-0.0334</v>
       </c>
       <c r="E2">
-        <v>0.1438</v>
+        <v>0.1203</v>
       </c>
       <c r="F2">
-        <v>-0.1177</v>
+        <v>-0.09520000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -461,19 +461,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.0106</v>
+        <v>0.0175</v>
       </c>
       <c r="C3">
-        <v>0.0106</v>
+        <v>0.0175</v>
       </c>
       <c r="D3">
-        <v>0.0157</v>
+        <v>0.0172</v>
       </c>
       <c r="E3">
-        <v>0.1964</v>
+        <v>0.1342</v>
       </c>
       <c r="F3">
-        <v>-0.3781</v>
+        <v>-0.1202</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -481,19 +481,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.0073</v>
+        <v>0.0247</v>
       </c>
       <c r="C4">
-        <v>0.0073</v>
+        <v>0.0247</v>
       </c>
       <c r="D4">
-        <v>0.0054</v>
+        <v>0.0273</v>
       </c>
       <c r="E4">
-        <v>0.1344</v>
+        <v>0.1275</v>
       </c>
       <c r="F4">
-        <v>-0.1247</v>
+        <v>-0.074</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -501,19 +501,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.0083</v>
+        <v>0.0187</v>
       </c>
       <c r="C5">
-        <v>0.0083</v>
+        <v>0.0187</v>
       </c>
       <c r="D5">
-        <v>0.0145</v>
+        <v>0.014</v>
       </c>
       <c r="E5">
-        <v>0.1099</v>
+        <v>0.168</v>
       </c>
       <c r="F5">
-        <v>-0.1902</v>
+        <v>-0.0649</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -521,19 +521,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>-0.0587</v>
+        <v>0.0559</v>
       </c>
       <c r="C6">
-        <v>-0.0587</v>
+        <v>0.0559</v>
       </c>
       <c r="D6">
-        <v>-0.06370000000000001</v>
+        <v>0.0585</v>
       </c>
       <c r="E6">
-        <v>0.0508</v>
+        <v>0.1627</v>
       </c>
       <c r="F6">
-        <v>-0.1933</v>
+        <v>-0.0144</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -541,19 +541,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>-0.0576</v>
+        <v>0.0525</v>
       </c>
       <c r="C7">
-        <v>-0.0576</v>
+        <v>0.0525</v>
       </c>
       <c r="D7">
-        <v>-0.06</v>
+        <v>0.0557</v>
       </c>
       <c r="E7">
-        <v>0.07530000000000001</v>
+        <v>0.1017</v>
       </c>
       <c r="F7">
-        <v>-0.1859</v>
+        <v>-0.0305</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -561,19 +561,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.0433</v>
+        <v>-0.0052</v>
       </c>
       <c r="C8">
-        <v>0.0433</v>
+        <v>-0.0052</v>
       </c>
       <c r="D8">
-        <v>0.0461</v>
+        <v>-0.006</v>
       </c>
       <c r="E8">
-        <v>0.1274</v>
+        <v>0.0535</v>
       </c>
       <c r="F8">
-        <v>-0.1028</v>
+        <v>-0.0669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
only pasture function is added
</commit_message>
<xml_diff>
--- a/Summary_2022-08-28.xlsx
+++ b/Summary_2022-08-28.xlsx
@@ -441,19 +441,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-0.007900000000000001</v>
+        <v>0.0241</v>
       </c>
       <c r="C2">
-        <v>-0.007900000000000001</v>
+        <v>0.0241</v>
       </c>
       <c r="D2">
-        <v>-0.0334</v>
+        <v>0.0328</v>
       </c>
       <c r="E2">
-        <v>0.1203</v>
+        <v>0.1438</v>
       </c>
       <c r="F2">
-        <v>-0.09520000000000001</v>
+        <v>-0.1177</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -461,19 +461,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.0175</v>
+        <v>0.0106</v>
       </c>
       <c r="C3">
-        <v>0.0175</v>
+        <v>0.0106</v>
       </c>
       <c r="D3">
-        <v>0.0172</v>
+        <v>0.0157</v>
       </c>
       <c r="E3">
-        <v>0.1342</v>
+        <v>0.1964</v>
       </c>
       <c r="F3">
-        <v>-0.1202</v>
+        <v>-0.3781</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -481,19 +481,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.0247</v>
+        <v>0.0073</v>
       </c>
       <c r="C4">
-        <v>0.0247</v>
+        <v>0.0073</v>
       </c>
       <c r="D4">
-        <v>0.0273</v>
+        <v>0.0054</v>
       </c>
       <c r="E4">
-        <v>0.1275</v>
+        <v>0.1344</v>
       </c>
       <c r="F4">
-        <v>-0.074</v>
+        <v>-0.1247</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -501,19 +501,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.0187</v>
+        <v>0.0083</v>
       </c>
       <c r="C5">
-        <v>0.0187</v>
+        <v>0.0083</v>
       </c>
       <c r="D5">
-        <v>0.014</v>
+        <v>0.0145</v>
       </c>
       <c r="E5">
-        <v>0.168</v>
+        <v>0.1099</v>
       </c>
       <c r="F5">
-        <v>-0.0649</v>
+        <v>-0.1902</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -521,19 +521,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.0559</v>
+        <v>-0.0587</v>
       </c>
       <c r="C6">
-        <v>0.0559</v>
+        <v>-0.0587</v>
       </c>
       <c r="D6">
-        <v>0.0585</v>
+        <v>-0.06370000000000001</v>
       </c>
       <c r="E6">
-        <v>0.1627</v>
+        <v>0.0508</v>
       </c>
       <c r="F6">
-        <v>-0.0144</v>
+        <v>-0.1933</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -541,19 +541,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.0525</v>
+        <v>-0.0576</v>
       </c>
       <c r="C7">
-        <v>0.0525</v>
+        <v>-0.0576</v>
       </c>
       <c r="D7">
-        <v>0.0557</v>
+        <v>-0.06</v>
       </c>
       <c r="E7">
-        <v>0.1017</v>
+        <v>0.07530000000000001</v>
       </c>
       <c r="F7">
-        <v>-0.0305</v>
+        <v>-0.1859</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -561,19 +561,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>-0.0052</v>
+        <v>0.0433</v>
       </c>
       <c r="C8">
-        <v>-0.0052</v>
+        <v>0.0433</v>
       </c>
       <c r="D8">
-        <v>-0.006</v>
+        <v>0.0461</v>
       </c>
       <c r="E8">
-        <v>0.0535</v>
+        <v>0.1274</v>
       </c>
       <c r="F8">
-        <v>-0.0669</v>
+        <v>-0.1028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>